<commit_message>
Reran analy, worked on figures for upcoming meeting
</commit_message>
<xml_diff>
--- a/tables/PH Seasons Tables.xlsx
+++ b/tables/PH Seasons Tables.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewpierson/Desktop/Heloderma Spatial/Heloderma Spatial/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewpierson/Desktop/Heloderma Spatial/Heloderma Spatial/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899DDF6B-3125-EE4E-9EFA-1C4C074201A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A9A5FB-5ED7-6D4E-ACE8-F6C6A93FC062}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="21060" windowHeight="10480" xr2:uid="{1F865958-604C-9443-AB2A-5B6BD2F9A602}"/>
+    <workbookView xWindow="0" yWindow="2680" windowWidth="21060" windowHeight="10480" xr2:uid="{1F865958-604C-9443-AB2A-5B6BD2F9A602}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -412,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -423,65 +425,64 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -799,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{367DDD8F-6FA1-8F45-A740-4916F57893D4}">
   <dimension ref="A2:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:D18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -811,52 +812,52 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="K2" s="16" t="s">
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="K2" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="12" t="s">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="K3" s="17" t="s">
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="K3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="18" t="s">
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
     </row>
     <row r="4" spans="1:17" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -874,7 +875,7 @@
       <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="10" t="s">
         <v>0</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -886,25 +887,25 @@
       <c r="I4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="20" t="s">
+      <c r="L4" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="M4" s="20" t="s">
+      <c r="M4" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="20" t="s">
+      <c r="N4" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O4" s="21" t="s">
+      <c r="O4" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="P4" s="20" t="s">
+      <c r="P4" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="Q4" s="20" t="s">
+      <c r="Q4" s="12" t="s">
         <v>42</v>
       </c>
     </row>
@@ -922,7 +923,7 @@
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="9"/>
+      <c r="F5" s="8"/>
       <c r="G5" s="1" t="s">
         <v>22</v>
       </c>
@@ -935,22 +936,22 @@
       <c r="K5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L5" s="22">
+      <c r="L5" s="14">
         <v>31.6</v>
       </c>
-      <c r="M5" s="22">
+      <c r="M5" s="14">
         <v>0.74</v>
       </c>
-      <c r="N5" s="22">
+      <c r="N5" s="14">
         <v>0.46</v>
       </c>
-      <c r="O5" s="23">
+      <c r="O5" s="15">
         <v>49</v>
       </c>
-      <c r="P5" s="24">
+      <c r="P5" s="16">
         <v>0.13</v>
       </c>
-      <c r="Q5" s="24">
+      <c r="Q5" s="16">
         <v>0.89</v>
       </c>
     </row>
@@ -966,7 +967,7 @@
       <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="9"/>
+      <c r="F6" s="8"/>
       <c r="G6" s="1" t="s">
         <v>23</v>
       </c>
@@ -979,22 +980,22 @@
       <c r="K6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L6" s="22">
+      <c r="L6" s="14">
         <v>31.6</v>
       </c>
-      <c r="M6" s="22">
+      <c r="M6" s="14">
         <v>-1.8</v>
       </c>
-      <c r="N6" s="22">
+      <c r="N6" s="14">
         <v>0.08</v>
       </c>
-      <c r="O6" s="23">
+      <c r="O6" s="15">
         <v>47.2</v>
       </c>
-      <c r="P6" s="24">
+      <c r="P6" s="16">
         <v>-3.65</v>
       </c>
-      <c r="Q6" s="25">
+      <c r="Q6" s="17">
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
@@ -1010,7 +1011,7 @@
       <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="9"/>
+      <c r="F7" s="8"/>
       <c r="G7" s="1" t="s">
         <v>24</v>
       </c>
@@ -1023,22 +1024,22 @@
       <c r="K7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L7" s="22">
+      <c r="L7" s="14">
         <v>31.5</v>
       </c>
-      <c r="M7" s="22">
+      <c r="M7" s="14">
         <v>0.44</v>
       </c>
-      <c r="N7" s="22">
+      <c r="N7" s="14">
         <v>0.65</v>
       </c>
-      <c r="O7" s="23">
+      <c r="O7" s="15">
         <v>47.1</v>
       </c>
-      <c r="P7" s="24">
+      <c r="P7" s="16">
         <v>-1.44</v>
       </c>
-      <c r="Q7" s="24">
+      <c r="Q7" s="16">
         <v>0.15</v>
       </c>
     </row>
@@ -1048,29 +1049,29 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="9"/>
+      <c r="F8" s="8"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="K8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L8" s="26">
+      <c r="L8" s="18">
         <v>31.9</v>
       </c>
-      <c r="M8" s="26">
+      <c r="M8" s="18">
         <v>0.03</v>
       </c>
-      <c r="N8" s="26">
+      <c r="N8" s="18">
         <v>0.97</v>
       </c>
-      <c r="O8" s="27">
+      <c r="O8" s="19">
         <v>48.9</v>
       </c>
-      <c r="P8" s="26">
+      <c r="P8" s="18">
         <v>0.65</v>
       </c>
-      <c r="Q8" s="26">
+      <c r="Q8" s="18">
         <v>0.51</v>
       </c>
     </row>
@@ -1086,7 +1087,7 @@
       <c r="E9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="9"/>
+      <c r="F9" s="8"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
         <v>31</v>
@@ -1105,7 +1106,7 @@
       <c r="E10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="9"/>
+      <c r="F10" s="8"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
         <v>32</v>
@@ -1124,7 +1125,7 @@
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="9"/>
+      <c r="F11" s="8"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
         <v>33</v>
@@ -1139,7 +1140,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="9"/>
+      <c r="F12" s="8"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1154,7 +1155,7 @@
       <c r="E13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="9"/>
+      <c r="F13" s="8"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1" t="s">
@@ -1169,7 +1170,7 @@
       <c r="E14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="9"/>
+      <c r="F14" s="8"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1" t="s">
@@ -1184,7 +1185,7 @@
       <c r="E15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="10"/>
+      <c r="F15" s="9"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6" t="s">
@@ -1206,93 +1207,92 @@
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="28" t="s">
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+    </row>
+    <row r="19" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="22">
+      <c r="B20" s="14">
         <v>87.7</v>
       </c>
-      <c r="C20" s="30">
+      <c r="C20" s="22">
         <v>-0.3</v>
       </c>
-      <c r="D20" s="30">
+      <c r="D20" s="22">
         <v>0.76</v>
       </c>
-      <c r="E20" s="8"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="22">
+      <c r="B21" s="14">
         <v>88.3</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21" s="14">
         <v>2.35</v>
       </c>
-      <c r="D21" s="31">
+      <c r="D21" s="23">
         <v>0.02</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="22">
+      <c r="B22" s="14">
         <v>87.2</v>
       </c>
-      <c r="C22" s="22">
+      <c r="C22" s="14">
         <v>4.8099999999999996</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="26">
+      <c r="B23" s="18">
         <v>89.4</v>
       </c>
-      <c r="C23" s="26">
+      <c r="C23" s="18">
         <v>-0.92</v>
       </c>
-      <c r="D23" s="26">
+      <c r="D23" s="18">
         <v>0.35</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="K2:Q2"/>
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="K3:N3"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="K2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>